<commit_message>
Polygon update (code) + pptx update + requirements
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73DCBE6-29AD-41CF-B0E6-A7E0D5F780D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9E5AC-8E6F-4FFD-9C6E-9ADAC5DB2A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" activeTab="4" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="1" activeTab="4" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="STBL IHM" sheetId="3" r:id="rId3"/>
     <sheet name="STBL OPs" sheetId="4" r:id="rId4"/>
     <sheet name="STBL EF" sheetId="7" r:id="rId5"/>
-    <sheet name="Capella to python" sheetId="6" r:id="rId6"/>
+    <sheet name="Specific requirements" sheetId="8" r:id="rId6"/>
+    <sheet name="Capella to python" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,150 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="13">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="13">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="165">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -239,9 +382,6 @@
   </si>
   <si>
     <t>1- Panneau global</t>
-  </si>
-  <si>
-    <t>(image)</t>
   </si>
   <si>
     <t>Le système doit posseder tous les champs de renseignement afin de lancer une simulation</t>
@@ -539,6 +679,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Diagramme des classes</t>
+  </si>
+  <si>
+    <t>Herite de</t>
+  </si>
+  <si>
+    <t>Diagramme de séquence</t>
+  </si>
+  <si>
+    <t>Diagramme Structurel</t>
   </si>
 </sst>
 </file>
@@ -623,7 +775,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -646,12 +798,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -661,6 +807,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
@@ -668,7 +824,26 @@
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -681,345 +856,143 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>88303</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>5194589</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CEF779D-3179-4129-9D6E-AAD2981B70E7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1383703" y="5114925"/>
-          <a:ext cx="5106286" cy="3238500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>53867</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>271462</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133145</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19E981F3-92F4-4565-B584-8227A656B546}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8688280" y="5091112"/>
-          <a:ext cx="2708178" cy="3238500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>555951</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4841237</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1B1A9D-CADC-43F4-A84D-1BEE2EB247C7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1851351" y="9767887"/>
-          <a:ext cx="4285286" cy="3238500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>98586</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>215585</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>91913</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28AC421A-0C4D-4321-8334-68B70D63D1CE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7358064" y="10757061"/>
-          <a:ext cx="5416234" cy="1260152"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1140123</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4199917</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CA334A0-A5A0-42D8-9961-1F74238C3758}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2435523" y="14578011"/>
-          <a:ext cx="3059794" cy="3238500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19089</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161949</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Image 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249FDB4B-FA00-595F-61FC-B022F0A58130}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1295400" y="476250"/>
-          <a:ext cx="5415002" cy="3238524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>80982</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161949</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Image 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2672A7B-73E5-C91B-2785-3EE0BDBCBA77}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8634413" y="476250"/>
-          <a:ext cx="2709882" cy="3238524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="13">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+</richValueRels>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F34F414-368F-4C6C-8624-6921052506CF}" name="Tableau2" displayName="Tableau2" ref="B2:D31" totalsRowShown="0">
+  <autoFilter ref="B2:D31" xr:uid="{3F34F414-368F-4C6C-8624-6921052506CF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0BD36610-BA62-4E4C-B5F8-FB54B58D1574}" name="Req_ID"/>
+    <tableColumn id="2" xr3:uid="{116882AE-2837-4886-B8DB-A9479BDE3D53}" name=" "/>
+    <tableColumn id="3" xr3:uid="{194A5147-F522-4571-9A4A-AAFF9A1B875E}" name="Hérite de"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{95711F4B-3FCA-47EE-B296-A4EF2D168774}" name="Tableau3" displayName="Tableau3" ref="C2:E80" totalsRowShown="0">
   <autoFilter ref="C2:E80" xr:uid="{95711F4B-3FCA-47EE-B296-A4EF2D168774}"/>
   <tableColumns count="3">
@@ -1027,7 +1000,19 @@
     <tableColumn id="2" xr3:uid="{F4FC994E-830B-4BEB-9E7F-1146B6283D70}" name=" "/>
     <tableColumn id="3" xr3:uid="{12369DCF-8882-4534-8CE2-E895EB53915D}" name="Hérite de"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB4C5999-D4C1-4F13-B039-B0595723EB21}" name="Tableau1" displayName="Tableau1" ref="C1:E12" totalsRowShown="0">
+  <autoFilter ref="C1:E12" xr:uid="{DB4C5999-D4C1-4F13-B039-B0595723EB21}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3651D10D-1D37-4920-B7D3-3AB77244F6F7}" name="Req_ID"/>
+    <tableColumn id="2" xr3:uid="{81CEAE99-8BE7-494E-A39A-DC833771F5D8}" name=" " dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{9EC6EE28-DFD8-4593-9605-55A6851859F1}" name="Herite de"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1385,7 +1370,7 @@
   <dimension ref="B3:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1403,7 +1388,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1411,19 +1396,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="10"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="10"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1431,25 +1416,25 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="11"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="11"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="11"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1457,19 +1442,19 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="10"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="10"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1477,31 +1462,31 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="11"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="11"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="11"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="11"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1509,19 +1494,19 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="10"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="10"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="10"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
@@ -1541,191 +1526,238 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B92590A-076F-48BF-A173-5735EF4A4DCA}">
-  <dimension ref="B2:P97"/>
+  <dimension ref="B2:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="75.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="31.53125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="72.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
       <c r="C2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="C3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="O3" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C4" s="3" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="C7" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C8" s="16" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="O3" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="P4" s="3"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.45">
       <c r="P9" s="3"/>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.45">
-      <c r="P14" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="P19" s="3" t="s">
-        <v>66</v>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="C11" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C12" s="16" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="C15" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C16" s="16" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="C19" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C20" s="16" t="e" vm="5">
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B21">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B22">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="P24" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C27" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>75</v>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="C25" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C26" s="16" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="C29" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C30" s="3"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C30" s="16" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C35" s="3"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>73</v>
-      </c>
-      <c r="E46">
-        <v>7</v>
-      </c>
-      <c r="F46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B47">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>74</v>
-      </c>
-      <c r="E47">
-        <v>8</v>
-      </c>
-      <c r="F47" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C52" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B71">
-        <v>9</v>
-      </c>
-      <c r="C71" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71">
-        <v>13</v>
-      </c>
-      <c r="F71" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B72">
-        <v>10</v>
-      </c>
-      <c r="C72" t="s">
-        <v>80</v>
-      </c>
-      <c r="E72">
-        <v>14</v>
-      </c>
-      <c r="F72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B73">
-        <v>11</v>
-      </c>
-      <c r="C73" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B74">
-        <v>12</v>
-      </c>
-      <c r="C74" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C78" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B97">
-        <v>15</v>
-      </c>
-      <c r="C97" t="s">
-        <v>87</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1733,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2DAA38-DBDF-46E2-B419-F6451EE365BA}">
   <dimension ref="C2:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1747,13 +1779,13 @@
   <sheetData>
     <row r="2" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
       <c r="C2" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>161</v>
-      </c>
       <c r="E2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
@@ -1766,8 +1798,8 @@
       <c r="C4">
         <v>16</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>89</v>
+      <c r="D4" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.45">
@@ -1775,8 +1807,8 @@
         <f>C4+1</f>
         <v>17</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>90</v>
+      <c r="D5" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="156.75" x14ac:dyDescent="0.45">
@@ -1784,8 +1816,8 @@
         <f t="shared" ref="C6:C9" si="0">C5+1</f>
         <v>18</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>91</v>
+      <c r="D6" s="11" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="42.75" x14ac:dyDescent="0.45">
@@ -1793,8 +1825,8 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>92</v>
+      <c r="D7" s="11" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.45">
@@ -1802,8 +1834,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>93</v>
+      <c r="D8" s="10" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.45">
@@ -1811,365 +1843,365 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>94</v>
+      <c r="D9" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C11">
         <v>22</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>95</v>
+      <c r="D11" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C12">
         <v>23</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>96</v>
+      <c r="D12" s="12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C13">
         <v>24</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>97</v>
+      <c r="D13" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C14">
         <v>25</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>98</v>
+      <c r="D14" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C15">
         <v>26</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>100</v>
+      <c r="D15" s="12" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C16">
         <v>27</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>99</v>
+      <c r="D16" s="12" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>28</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>101</v>
+      <c r="D17" s="12" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18">
         <v>29</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>104</v>
+      <c r="D18" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C19">
         <v>30</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>103</v>
+      <c r="D19" s="12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C20">
         <v>31</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>102</v>
+      <c r="D20" s="12" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C21">
         <v>32</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>105</v>
+      <c r="D21" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C22">
         <v>33</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>106</v>
+      <c r="D22" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C23">
         <v>34</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>107</v>
+      <c r="D23" s="12" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C24">
         <v>35</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>108</v>
+      <c r="D24" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C25">
         <v>36</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>109</v>
+      <c r="D25" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C26">
         <v>37</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>110</v>
+      <c r="D26" s="12" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D27" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C28">
         <v>38</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>111</v>
+      <c r="D28" s="10" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C29">
         <v>39</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>112</v>
+      <c r="D29" s="10" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C30">
         <v>40</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>113</v>
+      <c r="D30" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C31">
         <v>41</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>114</v>
+      <c r="D31" s="10" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C32">
         <v>42</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>115</v>
+      <c r="D32" s="10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C33">
         <v>43</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>116</v>
+      <c r="D33" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C34">
         <v>44</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>106</v>
+      <c r="D34" s="10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C35">
         <v>45</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>117</v>
+      <c r="D35" s="10" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C36">
         <v>46</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>118</v>
+      <c r="D36" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C37">
         <v>47</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>119</v>
+      <c r="D37" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C38">
         <v>48</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>120</v>
+      <c r="D38" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D39" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C40">
         <v>49</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>128</v>
+      <c r="D40" s="10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C41">
         <v>50</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>129</v>
+      <c r="D41" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C42">
         <v>51</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>130</v>
+      <c r="D42" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C43">
         <v>52</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>131</v>
+      <c r="D43" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C44">
         <v>53</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>132</v>
+      <c r="D44" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C45">
         <v>54</v>
       </c>
-      <c r="D45" s="12" t="s">
-        <v>121</v>
+      <c r="D45" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C46">
         <v>55</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>122</v>
+      <c r="D46" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C47">
         <v>56</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>123</v>
+      <c r="D47" s="10" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C48">
         <v>57</v>
       </c>
-      <c r="D48" s="12" t="s">
-        <v>133</v>
+      <c r="D48" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C49">
         <v>58</v>
       </c>
-      <c r="D49" s="12" t="s">
-        <v>134</v>
+      <c r="D49" s="10" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C50">
         <v>59</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>135</v>
+      <c r="D50" s="10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C51">
         <v>60</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>124</v>
+      <c r="D51" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C52">
         <v>61</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>125</v>
+      <c r="D52" s="10" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C53">
         <v>62</v>
       </c>
-      <c r="D53" s="12" t="s">
-        <v>126</v>
+      <c r="D53" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C54">
         <v>63</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>127</v>
+      <c r="D54" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D55" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.45">
@@ -2177,7 +2209,7 @@
         <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.45">
@@ -2185,7 +2217,7 @@
         <v>65</v>
       </c>
       <c r="D57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.45">
@@ -2193,7 +2225,7 @@
         <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.45">
@@ -2201,7 +2233,7 @@
         <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.45">
@@ -2209,7 +2241,7 @@
         <v>68</v>
       </c>
       <c r="D60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.45">
@@ -2217,7 +2249,7 @@
         <v>69</v>
       </c>
       <c r="D61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.45">
@@ -2225,7 +2257,7 @@
         <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.45">
@@ -2233,7 +2265,7 @@
         <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.45">
@@ -2241,7 +2273,7 @@
         <v>72</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.45">
@@ -2249,12 +2281,12 @@
         <v>73</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D66" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.45">
@@ -2262,7 +2294,7 @@
         <v>74</v>
       </c>
       <c r="D67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.45">
@@ -2270,7 +2302,7 @@
         <v>75</v>
       </c>
       <c r="D68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.45">
@@ -2278,7 +2310,7 @@
         <v>76</v>
       </c>
       <c r="D69" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.45">
@@ -2286,7 +2318,7 @@
         <v>77</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.45">
@@ -2294,7 +2326,7 @@
         <v>78</v>
       </c>
       <c r="D71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.45">
@@ -2302,7 +2334,7 @@
         <v>79</v>
       </c>
       <c r="D72" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.45">
@@ -2310,7 +2342,7 @@
         <v>80</v>
       </c>
       <c r="D73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.45">
@@ -2318,12 +2350,12 @@
         <v>81</v>
       </c>
       <c r="D74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D75" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.45">
@@ -2331,7 +2363,7 @@
         <v>82</v>
       </c>
       <c r="D76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.45">
@@ -2339,7 +2371,7 @@
         <v>83</v>
       </c>
       <c r="D77" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.45">
@@ -2347,7 +2379,7 @@
         <v>84</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.45">
@@ -2355,7 +2387,7 @@
         <v>85</v>
       </c>
       <c r="D79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.45">
@@ -2363,7 +2395,7 @@
         <v>86</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2376,10 +2408,135 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CA02E7-6F95-445A-956A-4099969DE617}">
+  <dimension ref="C1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C1" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D2" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="C3">
+        <v>87</v>
+      </c>
+      <c r="D3" s="15" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D4" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="C5">
+        <v>88</v>
+      </c>
+      <c r="D5" s="15" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D6" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="C7">
+        <v>89</v>
+      </c>
+      <c r="D7" s="15" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="C8">
+        <v>90</v>
+      </c>
+      <c r="D8" s="15" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="C9">
+        <v>91</v>
+      </c>
+      <c r="D9" s="15" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="C10">
+        <v>92</v>
+      </c>
+      <c r="D10" s="15" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="D20" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2388,12 +2545,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605C9B40-AC35-4309-ABDD-F2697D598540}">
   <dimension ref="A2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2411,7 +2568,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="13" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2420,21 +2577,21 @@
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2443,21 +2600,21 @@
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="11"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2466,21 +2623,21 @@
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2489,21 +2646,21 @@
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="11"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2512,35 +2669,35 @@
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="10"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="10"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="10"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -2549,21 +2706,21 @@
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2572,14 +2729,14 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="10"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="10"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
GT on main map + save&import correction for area
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9E5AC-8E6F-4FFD-9C6E-9ADAC5DB2A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D1261C-D9F5-490B-8D19-DB93E74688F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="1" activeTab="4" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="2" activeTab="3" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="183">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -691,6 +691,60 @@
   </si>
   <si>
     <t>Diagramme Structurel</t>
+  </si>
+  <si>
+    <t>tab1-&gt; add_satellite-&gt;init_sat</t>
+  </si>
+  <si>
+    <t>tab1-&gt; add_satellite-&gt;init_orb</t>
+  </si>
+  <si>
+    <t>tab1-&gt; add_satellite</t>
+  </si>
+  <si>
+    <t>tab2-&gt;add_constellation-&gt;init_constellation</t>
+  </si>
+  <si>
+    <t>tab3-&gt;add_poi-&gt;init_poi</t>
+  </si>
+  <si>
+    <t>tab3-&gt;add_poi-&gt;init_poi-&gt;findtimezone</t>
+  </si>
+  <si>
+    <t>tab5-&gt;comb_const_upd</t>
+  </si>
+  <si>
+    <t>tab5-&gt;ass_poi_mission</t>
+  </si>
+  <si>
+    <t>tab5-&gt;ass_gs_mission</t>
+  </si>
+  <si>
+    <t>tab5</t>
+  </si>
+  <si>
+    <t>tab3</t>
+  </si>
+  <si>
+    <t>tab2</t>
+  </si>
+  <si>
+    <t>tab3-&gt;add_gs-&gt;init_gs</t>
+  </si>
+  <si>
+    <t>tab5-&gt;add_mission-&gt;init_mission</t>
+  </si>
+  <si>
+    <t>calcul_traj-&gt;orbital_element_to_state_vector</t>
+  </si>
+  <si>
+    <t>calcul_traj</t>
+  </si>
+  <si>
+    <t>calcul_traj-&gt;runge_kutta_4</t>
+  </si>
+  <si>
+    <t>Le système doit afficher la trace au sol du satellite</t>
   </si>
 </sst>
 </file>
@@ -775,7 +829,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -791,7 +845,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -807,15 +860,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -993,8 +1046,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{95711F4B-3FCA-47EE-B296-A4EF2D168774}" name="Tableau3" displayName="Tableau3" ref="C2:E80" totalsRowShown="0">
-  <autoFilter ref="C2:E80" xr:uid="{95711F4B-3FCA-47EE-B296-A4EF2D168774}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{95711F4B-3FCA-47EE-B296-A4EF2D168774}" name="Tableau3" displayName="Tableau3" ref="C2:E82" totalsRowShown="0">
+  <autoFilter ref="C2:E82" xr:uid="{95711F4B-3FCA-47EE-B296-A4EF2D168774}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F6994145-DD36-49A6-92AB-F922F404692C}" name="Req_ID"/>
     <tableColumn id="2" xr3:uid="{F4FC994E-830B-4BEB-9E7F-1146B6283D70}" name=" "/>
@@ -1388,7 +1441,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1396,19 +1449,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="13"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="13"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1416,25 +1469,25 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="14"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1442,19 +1495,19 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="13"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1462,31 +1515,31 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="14"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="14"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="14"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="14"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1494,19 +1547,19 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="13"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="13"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="13"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
@@ -1545,7 +1598,7 @@
       <c r="B2" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>160</v>
       </c>
       <c r="D2" t="s">
@@ -1553,10 +1606,10 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1583,12 +1636,12 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C8" s="16" t="e" vm="2">
+      <c r="C8" s="13" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1610,12 +1663,12 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C12" s="16" t="e" vm="3">
+      <c r="C12" s="13" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1637,12 +1690,12 @@
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C16" s="16" t="e" vm="4">
+      <c r="C16" s="13" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1663,13 +1716,13 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>77</v>
       </c>
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C20" s="16" t="e" vm="5">
+      <c r="C20" s="13" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1707,12 +1760,12 @@
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C26" s="16" t="e" vm="6">
+      <c r="C26" s="13" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1733,12 +1786,12 @@
       </c>
     </row>
     <row r="29" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C30" s="16" t="e" vm="7">
+      <c r="C30" s="13" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1763,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2DAA38-DBDF-46E2-B419-F6451EE365BA}">
-  <dimension ref="C2:E80"/>
+  <dimension ref="C2:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1778,10 +1831,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>160</v>
       </c>
       <c r="E2" t="s">
@@ -1789,8 +1842,8 @@
       </c>
     </row>
     <row r="3" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1798,7 +1851,7 @@
       <c r="C4">
         <v>16</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1807,7 +1860,7 @@
         <f>C4+1</f>
         <v>17</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1816,7 +1869,7 @@
         <f t="shared" ref="C6:C9" si="0">C5+1</f>
         <v>18</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1825,7 +1878,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1834,7 +1887,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1843,13 +1896,13 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1857,7 +1910,7 @@
       <c r="C11">
         <v>22</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1865,7 +1918,7 @@
       <c r="C12">
         <v>23</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1873,7 +1926,7 @@
       <c r="C13">
         <v>24</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1881,7 +1934,7 @@
       <c r="C14">
         <v>25</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1889,7 +1942,7 @@
       <c r="C15">
         <v>26</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1897,7 +1950,7 @@
       <c r="C16">
         <v>27</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1905,7 +1958,7 @@
       <c r="C17">
         <v>28</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1913,7 +1966,7 @@
       <c r="C18">
         <v>29</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1921,7 +1974,7 @@
       <c r="C19">
         <v>30</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1929,7 +1982,7 @@
       <c r="C20">
         <v>31</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1937,7 +1990,7 @@
       <c r="C21">
         <v>32</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1945,7 +1998,7 @@
       <c r="C22">
         <v>33</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1953,7 +2006,7 @@
       <c r="C23">
         <v>34</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1961,7 +2014,7 @@
       <c r="C24">
         <v>35</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1969,7 +2022,7 @@
       <c r="C25">
         <v>36</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1977,12 +2030,12 @@
       <c r="C26">
         <v>37</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1990,7 +2043,7 @@
       <c r="C28">
         <v>38</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1998,7 +2051,7 @@
       <c r="C29">
         <v>39</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2006,7 +2059,7 @@
       <c r="C30">
         <v>40</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2014,7 +2067,7 @@
       <c r="C31">
         <v>41</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2022,7 +2075,7 @@
       <c r="C32">
         <v>42</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="9" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2030,7 +2083,7 @@
       <c r="C33">
         <v>43</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="9" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2038,7 +2091,7 @@
       <c r="C34">
         <v>44</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="9" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2046,7 +2099,7 @@
       <c r="C35">
         <v>45</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="9" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2054,7 +2107,7 @@
       <c r="C36">
         <v>46</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2062,7 +2115,7 @@
       <c r="C37">
         <v>47</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2070,12 +2123,12 @@
       <c r="C38">
         <v>48</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="9" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="39" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="8" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2083,7 +2136,7 @@
       <c r="C40">
         <v>49</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="9" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2091,7 +2144,7 @@
       <c r="C41">
         <v>50</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="9" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2099,7 +2152,7 @@
       <c r="C42">
         <v>51</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="9" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2107,7 +2160,7 @@
       <c r="C43">
         <v>52</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="9" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2115,7 +2168,7 @@
       <c r="C44">
         <v>53</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="9" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2123,7 +2176,7 @@
       <c r="C45">
         <v>54</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="9" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2131,7 +2184,7 @@
       <c r="C46">
         <v>55</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="9" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2139,7 +2192,7 @@
       <c r="C47">
         <v>56</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="9" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2147,7 +2200,7 @@
       <c r="C48">
         <v>57</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="9" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2155,7 +2208,7 @@
       <c r="C49">
         <v>58</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="9" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2163,7 +2216,7 @@
       <c r="C50">
         <v>59</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="9" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2171,7 +2224,7 @@
       <c r="C51">
         <v>60</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="9" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2179,7 +2232,7 @@
       <c r="C52">
         <v>61</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2187,7 +2240,7 @@
       <c r="C53">
         <v>62</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2195,12 +2248,12 @@
       <c r="C54">
         <v>63</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="8" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2285,7 +2338,7 @@
       </c>
     </row>
     <row r="66" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="8" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2354,7 +2407,7 @@
       </c>
     </row>
     <row r="75" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="8" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2396,6 +2449,14 @@
       </c>
       <c r="D80" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C81">
+        <v>87</v>
+      </c>
+      <c r="D81" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2410,8 +2471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CA02E7-6F95-445A-956A-4099969DE617}">
   <dimension ref="C1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2420,7 +2481,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>159</v>
       </c>
       <c r="D1" t="s">
@@ -2430,98 +2491,98 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D2" s="15" t="s">
+    <row r="2" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="D2" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="3" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="C3">
-        <v>87</v>
-      </c>
-      <c r="D3" s="15" t="e" vm="8">
+        <v>88</v>
+      </c>
+      <c r="D3" s="12" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D4" s="15" t="s">
+    <row r="4" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="D4" s="8" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="C5">
-        <v>88</v>
-      </c>
-      <c r="D5" s="15" t="e" vm="9">
+        <v>89</v>
+      </c>
+      <c r="D5" s="12" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D6" s="15" t="s">
+    <row r="6" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="D6" s="8" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="C7">
-        <v>89</v>
-      </c>
-      <c r="D7" s="15" t="e" vm="10">
+        <v>90</v>
+      </c>
+      <c r="D7" s="12" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="C8">
-        <v>90</v>
-      </c>
-      <c r="D8" s="15" t="e" vm="11">
+        <v>91</v>
+      </c>
+      <c r="D8" s="12" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="C9">
-        <v>91</v>
-      </c>
-      <c r="D9" s="15" t="e" vm="12">
+        <v>92</v>
+      </c>
+      <c r="D9" s="12" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
       <c r="C10">
-        <v>92</v>
-      </c>
-      <c r="D10" s="15" t="e" vm="13">
+        <v>93</v>
+      </c>
+      <c r="D10" s="12" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D11" s="15"/>
+      <c r="D11" s="12"/>
     </row>
     <row r="12" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D12" s="15"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D13" s="15"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D14" s="15"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D15" s="15"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D16" s="15"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D17" s="15"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D18" s="15"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D19" s="15"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="4:4" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="D20" s="15"/>
+      <c r="D20" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2536,7 +2597,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2550,177 +2611,218 @@
   <dimension ref="A2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="13"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="13"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="13"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="13"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2729,14 +2831,14 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="13"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Import and save function fixed
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D1261C-D9F5-490B-8D19-DB93E74688F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A60F7DD-02D2-4942-8989-8A18C3B74370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="2" activeTab="3" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="184">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -745,6 +745,9 @@
   </si>
   <si>
     <t>Le système doit afficher la trace au sol du satellite</t>
+  </si>
+  <si>
+    <t>pyinstaller --hidden-import "babel.numbers" main.py --onefile -w</t>
   </si>
 </sst>
 </file>
@@ -1366,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3161A64A-A6FA-48E0-B23C-B5A382045211}">
-  <dimension ref="B2:B8"/>
+  <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1410,6 +1413,11 @@
     <row r="8" spans="2:2" ht="31.5" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1818,7 +1826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2DAA38-DBDF-46E2-B419-F6451EE365BA}">
   <dimension ref="C2:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More bug fixing + TLE import option added
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A60F7DD-02D2-4942-8989-8A18C3B74370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361A30D7-25B4-4B0D-A2ED-8052096BC119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="7875" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="191">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -749,12 +749,34 @@
   <si>
     <t>pyinstaller --hidden-import "babel.numbers" main.py --onefile -w</t>
   </si>
+  <si>
+    <t>User Stories</t>
+  </si>
+  <si>
+    <t>ReqID</t>
+  </si>
+  <si>
+    <t>1- As a user, I want to be able to integrate data from real satellites 
+(telemetry, TLE) to compare simulations with real trajectories.</t>
+  </si>
+  <si>
+    <t>Le système doit afficher les données TLE dans un format compréhensible pour l'utilisateur</t>
+  </si>
+  <si>
+    <t>Le système doit permettre l'importation de données TLE (Two-Line Elements)</t>
+  </si>
+  <si>
+    <t>Le système doit verifier l'intégité de la TLE</t>
+  </si>
+  <si>
+    <t>Le système doit completer automatiquement les champs correspondant aux TLE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -787,6 +809,14 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -832,7 +862,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -872,6 +902,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1371,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3161A64A-A6FA-48E0-B23C-B5A382045211}">
   <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2602,14 +2635,54 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
-  <dimension ref="A1"/>
+  <dimension ref="A4:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="79.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
res step option added + more bug fixing
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361A30D7-25B4-4B0D-A2ED-8052096BC119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D799D78-CD92-4BFC-AD59-7AF0C29A9132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7875" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="6960" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="193">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -760,9 +760,6 @@
 (telemetry, TLE) to compare simulations with real trajectories.</t>
   </si>
   <si>
-    <t>Le système doit afficher les données TLE dans un format compréhensible pour l'utilisateur</t>
-  </si>
-  <si>
     <t>Le système doit permettre l'importation de données TLE (Two-Line Elements)</t>
   </si>
   <si>
@@ -770,6 +767,15 @@
   </si>
   <si>
     <t>Le système doit completer automatiquement les champs correspondant aux TLE</t>
+  </si>
+  <si>
+    <t>Le système doit pouvoir importer les TLE depuis internet</t>
+  </si>
+  <si>
+    <t>Le système doit avertir l'utilisateur si aucune TLE n'a été trouvée</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de renseigner le NORAD ID du satellite</t>
   </si>
 </sst>
 </file>
@@ -897,14 +903,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1482,7 +1488,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1490,19 +1496,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="14"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1510,25 +1516,25 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="15"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1536,19 +1542,19 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="14"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="14"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1556,31 +1562,31 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="15"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="15"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1588,19 +1594,19 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="14"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="14"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="14"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
@@ -2635,10 +2641,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
-  <dimension ref="A4:C9"/>
+  <dimension ref="A4:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2658,18 +2664,18 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -2679,7 +2685,17 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2711,7 +2727,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2722,7 +2738,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
@@ -2731,7 +2747,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
@@ -2740,7 +2756,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2751,7 +2767,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
@@ -2760,7 +2776,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="5" t="s">
         <v>55</v>
       </c>
@@ -2769,7 +2785,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2780,7 +2796,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
@@ -2789,7 +2805,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
@@ -2798,7 +2814,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2809,7 +2825,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -2818,7 +2834,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
@@ -2827,7 +2843,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2838,7 +2854,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
@@ -2847,7 +2863,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -2856,7 +2872,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
@@ -2865,7 +2881,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
@@ -2874,7 +2890,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -2885,7 +2901,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
@@ -2894,7 +2910,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="15"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
@@ -2903,7 +2919,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2912,14 +2928,14 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
bug correction + gs visibility function added
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D799D78-CD92-4BFC-AD59-7AF0C29A9132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC08189-523E-44E5-BBA1-29DCC98F9B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="7875" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="201">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -777,12 +777,38 @@
   <si>
     <t>Le système doit permettre à l'utilisateur de renseigner le NORAD ID du satellite</t>
   </si>
+  <si>
+    <t>2- As a user, I want to visualize satellite coverage areas to plan communication 
+or Earth observation missions.</t>
+  </si>
+  <si>
+    <t>Le système doit calculer la zone de couverture du/des satellites en fonction de l'orbite</t>
+  </si>
+  <si>
+    <t>Le système doit prendre en compte la fauchée et l'angle de dépointage du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit prendre en compte l'angle du zenith solaire pour une mission d'observation</t>
+  </si>
+  <si>
+    <t>Le système doit indiquer le nombre de couverture par jour d'un point d'interet</t>
+  </si>
+  <si>
+    <t>Le système doit indiquer au bout de combien de temps le satellite va revenir sur le point d'interet</t>
+  </si>
+  <si>
+    <t>Le système doit pouvoiur afficher le couloir d'observation du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit fournir des statistiques sur le nombre de revisite, la fréquence de revisite,
+le temps durant lequel le POI est visible</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,6 +849,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -868,7 +902,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -905,6 +939,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1106,6 +1146,18 @@
     <tableColumn id="1" xr3:uid="{3651D10D-1D37-4920-B7D3-3AB77244F6F7}" name="Req_ID"/>
     <tableColumn id="2" xr3:uid="{81CEAE99-8BE7-494E-A39A-DC833771F5D8}" name=" " dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{9EC6EE28-DFD8-4593-9605-55A6851859F1}" name="Herite de"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}" name="Tableau4" displayName="Tableau4" ref="A3:C19" totalsRowShown="0">
+  <autoFilter ref="A3:C19" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FB216FF5-5C23-45FE-9C7F-41D70FC25F5D}" name="ReqID"/>
+    <tableColumn id="2" xr3:uid="{27152B0E-8AF8-4A79-ABBC-8FF7DDD6B3A8}" name=" "/>
+    <tableColumn id="3" xr3:uid="{E069355D-77F7-4246-B980-15C9DAC72763}" name="Herite de"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1488,7 +1540,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1496,19 +1548,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1516,25 +1568,25 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="16"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="16"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="16"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1542,19 +1594,19 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="15"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="15"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1562,31 +1614,31 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="16"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="16"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="16"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1594,19 +1646,19 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="15"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="15"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="15"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
@@ -2641,26 +2693,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
-  <dimension ref="A4:C11"/>
+  <dimension ref="A3:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="B4" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -2669,37 +2726,119 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>94</v>
+      </c>
       <c r="B6" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>95</v>
+      </c>
       <c r="B7" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>96</v>
+      </c>
       <c r="B8" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>97</v>
+      </c>
       <c r="B9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>98</v>
+      </c>
       <c r="B10" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>99</v>
+      </c>
       <c r="B11" t="s">
         <v>188</v>
       </c>
     </row>
+    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>101</v>
+      </c>
+      <c r="B14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>102</v>
+      </c>
+      <c r="B15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>106</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2727,7 +2866,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2738,7 +2877,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
@@ -2747,7 +2886,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="15"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
@@ -2756,7 +2895,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2767,7 +2906,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
@@ -2776,7 +2915,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5" t="s">
         <v>55</v>
       </c>
@@ -2785,7 +2924,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2796,7 +2935,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="15"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
@@ -2805,7 +2944,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="15"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
@@ -2814,7 +2953,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2825,7 +2964,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="16"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -2834,7 +2973,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="16"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
@@ -2843,7 +2982,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2854,7 +2993,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="15"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
@@ -2863,7 +3002,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="15"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -2872,7 +3011,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="15"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
@@ -2881,7 +3020,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="15"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
@@ -2890,7 +3029,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -2901,7 +3040,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="16"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
@@ -2910,7 +3049,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
@@ -2919,7 +3058,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2928,14 +3067,14 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="15"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="15"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
result&simulation files moved + bug fixing
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC08189-523E-44E5-BBA1-29DCC98F9B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF07221-5C2E-4719-B8AC-B5529F1215F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7875" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="2" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="214">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -483,45 +483,18 @@
     <t>Le système doit permettre à l'utilisateur de rentrer le nom du satellite</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer la fauchée du satellite</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'angle de dépointage max du satellite</t>
-  </si>
-  <si>
     <t>Le système doit permettre à l'utilisateur de choisir la couleur du satellite</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'altitude du satellite</t>
-  </si>
-  <si>
     <t>Le système doit permettre à l'utilisateur de choisir le type de satellite</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'eccentricité de l'orbite du satellite</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'argument du perigée de l'orbite du satellite</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer le RAAN de l'orbite du satellite</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'inclinaison de l'orbite du satellite</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'anomalie vraie du satellite</t>
-  </si>
-  <si>
     <t>Le système doit informer l'utilisateur de données non conformes</t>
   </si>
   <si>
     <t>Le système doit interdire l'ajout du satellite si l'un des parametres est non conforme ou absent</t>
   </si>
   <si>
-    <t>Le système doit permettre la modification des parametre du satellite</t>
-  </si>
-  <si>
     <t>Le système doit permettre la suppression du satellite</t>
   </si>
   <si>
@@ -537,9 +510,6 @@
     <t>Le système doit permettre à l'utilisateur de rentrer le nombre total de plan orbitaux de la constellation</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer le facteur de phase de la constellation</t>
-  </si>
-  <si>
     <t>Le système doit permettre à l'utilisateur de choisir un satellite modele pour la constellation</t>
   </si>
   <si>
@@ -564,9 +534,6 @@
     <t>Le système doit permettre à l'utilisateur de dessiner manuellement une zone sur la carte</t>
   </si>
   <si>
-    <t>Le système doit interdire l'utilsateur de rentrer la longitude et la latitude si une zone est présente sur la carte</t>
-  </si>
-  <si>
     <t>Le système doit interdire l'ajout du POI/ZOI/GS si l'un des parametres est non conforme ou absent</t>
   </si>
   <si>
@@ -582,40 +549,16 @@
     <t>Le système doit permettre à l'utilisateur de rentrer le nom du POI/ZOI/GS</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer la latitude du POI/GS</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer la longitude du POI/GS</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentre l'altitude du POI/ZOI/GS</t>
-  </si>
-  <si>
     <t>Le système doit permettre à l'utilisateur de choisir la couleur du POI/ZOI/GS</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'élévation du GS</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer la bande passante du GS</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentre le débit du GS</t>
-  </si>
-  <si>
     <t>Le système doit permettre à l'utilisateur de rentrer le nom de la mission</t>
   </si>
   <si>
     <t>Le système doit permettre à l'utilisateur de rentrer la durée de la mission</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer le pas de temps de la mission</t>
-  </si>
-  <si>
     <t>Le système doit permettre à l'utilisateur de choisir le type de mission</t>
-  </si>
-  <si>
-    <t>Le système doit permettre à l'utilisateur de rentrer l'angle minimal du soleil par rapport au zenith</t>
   </si>
   <si>
     <t xml:space="preserve">Le système doit permettre à l'utilisateur de choisir un ou plusieurs POI/GS et de l'associer à la mission </t>
@@ -778,30 +721,136 @@
     <t>Le système doit permettre à l'utilisateur de renseigner le NORAD ID du satellite</t>
   </si>
   <si>
-    <t>2- As a user, I want to visualize satellite coverage areas to plan communication 
-or Earth observation missions.</t>
-  </si>
-  <si>
-    <t>Le système doit calculer la zone de couverture du/des satellites en fonction de l'orbite</t>
-  </si>
-  <si>
-    <t>Le système doit prendre en compte la fauchée et l'angle de dépointage du satellite</t>
-  </si>
-  <si>
-    <t>Le système doit prendre en compte l'angle du zenith solaire pour une mission d'observation</t>
-  </si>
-  <si>
-    <t>Le système doit indiquer le nombre de couverture par jour d'un point d'interet</t>
-  </si>
-  <si>
-    <t>Le système doit indiquer au bout de combien de temps le satellite va revenir sur le point d'interet</t>
-  </si>
-  <si>
-    <t>Le système doit pouvoiur afficher le couloir d'observation du satellite</t>
-  </si>
-  <si>
-    <t>Le système doit fournir des statistiques sur le nombre de revisite, la fréquence de revisite,
-le temps durant lequel le POI est visible</t>
+    <t>2- As a user, I want to obtain detailed information on satellite passes over specific geographical areas to plan observations or operations</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de choisir un satellite simulé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le système doit indiquer le nombre de passage au-dessus de la station sol/poi </t>
+  </si>
+  <si>
+    <t>Le système doit indiquer la taille de la donnée max envoyable (en Mo) pour chaque passage au-dessus
+ d'une station sol</t>
+  </si>
+  <si>
+    <t>Le système doit indiquer l'élévation du soleil (en °) moyenne pour chaque passage au-dessus d'un poi</t>
+  </si>
+  <si>
+    <t>Le système doit afficher l'élévation du soleil (en °) pour le poi concerné</t>
+  </si>
+  <si>
+    <t>Le système doit indiquer la durée de passage (en s) au-dessus de la station sol/poi</t>
+  </si>
+  <si>
+    <t>Le système doit afficher l'elevation (en °) entre la station sol/poi et le satellite choisi</t>
+  </si>
+  <si>
+    <t>Le système doit indiquer les intervalles de temps pour lesquels la station sol/poi est visible</t>
+  </si>
+  <si>
+    <t>Le système doit exporter les résultats précédents</t>
+  </si>
+  <si>
+    <t>3- As a user, I want to be able to adjust the time interval and resolution step for orbit propagation 
+calculations to strike a balance between accuracy and performance.</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de definir pas de temps de la simulation</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de chosir entre les 3 niveaux de résolution géométrique suivant:
+- 10 m
+- 50 m
+- 110 m</t>
+  </si>
+  <si>
+    <t>Le système doit indiquer le temps d'exécution du calcul</t>
+  </si>
+  <si>
+    <t>4- As a user, I want to be able to simulate satellite constellations to model satellite networks for 
+specific applications.</t>
+  </si>
+  <si>
+    <t>Le système doit afficher la constellation en 3D</t>
+  </si>
+  <si>
+    <t>Le système doit afficher la trace au sol de chaque satellite</t>
+  </si>
+  <si>
+    <t>Le système doit afficher la position des satellites sur la trace au sol à la fin de la simulation</t>
+  </si>
+  <si>
+    <t>Le système doit afficher la position des satellites en 3D à la fin de la simulation</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer les parametres suivant lors de la création 
+de la constellation : 
+- le nombre de satellite
+- le nombre de plan
+- la phase (en °) entre deux satellites sur deux plans successifs</t>
+  </si>
+  <si>
+    <t>5- As a user, I want to be able to export simulation data and visualizations for use in reports 
+or other analyses.</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer la fauchée (en km) du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'angle de dépointage max (en °) du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'altitude (en km) du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'eccentricité (entre 0 et 1) de l'orbite du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'inclinaison de l'orbite (en °) du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer le RAAN de l'orbite (en °) du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'argument du perigée de l'orbite (en °) du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'anomalie vraie (en °) du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre la modification des parametres du satellite</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer le facteur de phase (en °) de la constellation</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer la latitude (en degré décimal) du POI/GS</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer la longitude (en degré décimal) du POI/GS</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentre l'altitude (en m) du POI/ZOI/GS</t>
+  </si>
+  <si>
+    <t>Le système doit interdire l'utilsateur de rentrer la longitude (en degré décimal) et la latitude (en degré décimal) 
+si une zone est présente sur la carte</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'élévation (en °) du GS</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer la bande passante (MHz) du GS</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentre le débit (en Mb/s) du GS</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer le pas de temps (en s ou en jour) de la mission</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentrer l'angle minimal du soleil (en °) par rapport au zenith</t>
   </si>
 </sst>
 </file>
@@ -902,7 +951,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -951,6 +1000,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1152,8 +1204,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}" name="Tableau4" displayName="Tableau4" ref="A3:C19" totalsRowShown="0">
-  <autoFilter ref="A3:C19" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}" name="Tableau4" displayName="Tableau4" ref="A3:C39" totalsRowShown="0">
+  <autoFilter ref="A3:C39" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FB216FF5-5C23-45FE-9C7F-41D70FC25F5D}" name="ReqID"/>
     <tableColumn id="2" xr3:uid="{27152B0E-8AF8-4A79-ABBC-8FF7DDD6B3A8}" name=" "/>
@@ -1508,7 +1560,7 @@
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1695,13 +1747,13 @@
   <sheetData>
     <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="23.25" x14ac:dyDescent="0.45">
@@ -1917,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2DAA38-DBDF-46E2-B419-F6451EE365BA}">
   <dimension ref="C2:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1931,13 +1983,13 @@
   <sheetData>
     <row r="2" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
       <c r="C2" s="7" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
@@ -1964,7 +2016,7 @@
       </c>
     </row>
     <row r="6" spans="3:5" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="C6">
+      <c r="C6" s="19">
         <f t="shared" ref="C6:C9" si="0">C5+1</f>
         <v>18</v>
       </c>
@@ -2018,7 +2070,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>95</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.45">
@@ -2026,7 +2078,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.45">
@@ -2034,7 +2086,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.45">
@@ -2042,7 +2094,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.45">
@@ -2050,7 +2102,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.45">
@@ -2058,7 +2110,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.45">
@@ -2066,7 +2118,7 @@
         <v>29</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.45">
@@ -2074,7 +2126,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.45">
@@ -2082,7 +2134,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.45">
@@ -2090,7 +2142,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.45">
@@ -2098,7 +2150,7 @@
         <v>33</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.45">
@@ -2106,7 +2158,7 @@
         <v>34</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.45">
@@ -2114,7 +2166,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>107</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.45">
@@ -2122,7 +2174,7 @@
         <v>36</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.45">
@@ -2130,7 +2182,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
@@ -2143,7 +2195,7 @@
         <v>38</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.45">
@@ -2151,7 +2203,7 @@
         <v>39</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.45">
@@ -2159,7 +2211,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.45">
@@ -2167,7 +2219,7 @@
         <v>41</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>113</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.45">
@@ -2175,7 +2227,7 @@
         <v>42</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.45">
@@ -2183,7 +2235,7 @@
         <v>43</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.45">
@@ -2191,7 +2243,7 @@
         <v>44</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.45">
@@ -2199,7 +2251,7 @@
         <v>45</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.45">
@@ -2207,7 +2259,7 @@
         <v>46</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.45">
@@ -2215,7 +2267,7 @@
         <v>47</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.45">
@@ -2223,7 +2275,7 @@
         <v>48</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
@@ -2236,7 +2288,7 @@
         <v>49</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.45">
@@ -2244,7 +2296,7 @@
         <v>50</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.45">
@@ -2252,7 +2304,7 @@
         <v>51</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>129</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.45">
@@ -2260,7 +2312,7 @@
         <v>52</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>130</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.45">
@@ -2268,7 +2320,7 @@
         <v>53</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.45">
@@ -2276,7 +2328,7 @@
         <v>54</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.45">
@@ -2284,15 +2336,15 @@
         <v>55</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C47">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C47" s="9">
         <v>56</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>122</v>
+      <c r="D47" s="10" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.45">
@@ -2300,7 +2352,7 @@
         <v>57</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>132</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.45">
@@ -2308,7 +2360,7 @@
         <v>58</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>133</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.45">
@@ -2316,7 +2368,7 @@
         <v>59</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>134</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.45">
@@ -2324,7 +2376,7 @@
         <v>60</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.45">
@@ -2332,7 +2384,7 @@
         <v>61</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.45">
@@ -2340,7 +2392,7 @@
         <v>62</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.45">
@@ -2348,7 +2400,7 @@
         <v>63</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
@@ -2361,7 +2413,7 @@
         <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.45">
@@ -2369,7 +2421,7 @@
         <v>65</v>
       </c>
       <c r="D57" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.45">
@@ -2377,7 +2429,7 @@
         <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>137</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.45">
@@ -2385,7 +2437,7 @@
         <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.45">
@@ -2393,7 +2445,7 @@
         <v>68</v>
       </c>
       <c r="D60" t="s">
-        <v>139</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.45">
@@ -2401,7 +2453,7 @@
         <v>69</v>
       </c>
       <c r="D61" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.45">
@@ -2409,7 +2461,7 @@
         <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.45">
@@ -2417,7 +2469,7 @@
         <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.45">
@@ -2425,7 +2477,7 @@
         <v>72</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.45">
@@ -2433,7 +2485,7 @@
         <v>73</v>
       </c>
       <c r="D65" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
@@ -2446,7 +2498,7 @@
         <v>74</v>
       </c>
       <c r="D67" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.45">
@@ -2454,7 +2506,7 @@
         <v>75</v>
       </c>
       <c r="D68" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.45">
@@ -2462,7 +2514,7 @@
         <v>76</v>
       </c>
       <c r="D69" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.45">
@@ -2470,7 +2522,7 @@
         <v>77</v>
       </c>
       <c r="D70" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.45">
@@ -2478,7 +2530,7 @@
         <v>78</v>
       </c>
       <c r="D71" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.45">
@@ -2486,7 +2538,7 @@
         <v>79</v>
       </c>
       <c r="D72" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.45">
@@ -2494,7 +2546,7 @@
         <v>80</v>
       </c>
       <c r="D73" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.45">
@@ -2502,7 +2554,7 @@
         <v>81</v>
       </c>
       <c r="D74" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="3:4" ht="23.25" x14ac:dyDescent="0.45">
@@ -2515,7 +2567,7 @@
         <v>82</v>
       </c>
       <c r="D76" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.45">
@@ -2523,7 +2575,7 @@
         <v>83</v>
       </c>
       <c r="D77" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.45">
@@ -2531,7 +2583,7 @@
         <v>84</v>
       </c>
       <c r="D78" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.45">
@@ -2539,7 +2591,7 @@
         <v>85</v>
       </c>
       <c r="D79" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.45">
@@ -2547,7 +2599,7 @@
         <v>86</v>
       </c>
       <c r="D80" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.45">
@@ -2555,7 +2607,7 @@
         <v>87</v>
       </c>
       <c r="D81" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2581,18 +2633,18 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C1" s="7" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D2" s="8" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
@@ -2605,7 +2657,7 @@
     </row>
     <row r="4" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D4" s="8" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
@@ -2618,7 +2670,7 @@
     </row>
     <row r="6" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
       <c r="D6" s="8" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="23.25" x14ac:dyDescent="0.7">
@@ -2693,10 +2745,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
-  <dimension ref="A3:C19"/>
+  <dimension ref="A3:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2706,23 +2758,23 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.45">
       <c r="B4" s="8" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="14" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -2730,7 +2782,7 @@
         <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -2738,7 +2790,7 @@
         <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -2746,7 +2798,7 @@
         <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -2754,7 +2806,7 @@
         <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -2762,7 +2814,7 @@
         <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -2770,12 +2822,12 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="15" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -2783,7 +2835,7 @@
         <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -2791,7 +2843,7 @@
         <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -2799,7 +2851,7 @@
         <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -2807,7 +2859,7 @@
         <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -2815,29 +2867,125 @@
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>105</v>
-      </c>
-      <c r="B18" t="s">
-        <v>199</v>
+        <v>106</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>200</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A24" s="9">
+        <v>111</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A27" s="9">
+        <v>113</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>115</v>
+      </c>
+      <c r="B29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>116</v>
+      </c>
+      <c r="B30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>117</v>
+      </c>
+      <c r="B31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B32" s="14" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2873,7 +3021,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -2882,7 +3030,7 @@
         <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -2891,7 +3039,7 @@
         <v>59</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -2902,7 +3050,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -2911,7 +3059,7 @@
         <v>56</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -2920,7 +3068,7 @@
         <v>55</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -2931,7 +3079,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -2940,7 +3088,7 @@
         <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -2949,7 +3097,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -2960,7 +3108,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -2969,7 +3117,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -2978,7 +3126,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -2989,7 +3137,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -2998,7 +3146,7 @@
         <v>44</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -3007,7 +3155,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -3016,7 +3164,7 @@
         <v>42</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -3025,7 +3173,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -3036,7 +3184,7 @@
         <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -3045,7 +3193,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -3054,7 +3202,7 @@
         <v>37</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
bug fixing + attenuation model + data trasnmitted
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF07221-5C2E-4719-B8AC-B5529F1215F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CB7EB9-8DD4-4E2D-902F-9C3D466909A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="2" activeTab="5" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="13620" firstSheet="1" activeTab="3" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -844,13 +844,13 @@
     <t>Le système doit permettre à l'utilisateur de rentrer la bande passante (MHz) du GS</t>
   </si>
   <si>
-    <t>Le système doit permettre à l'utilisateur de rentre le débit (en Mb/s) du GS</t>
-  </si>
-  <si>
     <t>Le système doit permettre à l'utilisateur de rentrer le pas de temps (en s ou en jour) de la mission</t>
   </si>
   <si>
     <t>Le système doit permettre à l'utilisateur de rentrer l'angle minimal du soleil (en °) par rapport au zenith</t>
+  </si>
+  <si>
+    <t>Le système doit permettre à l'utilisateur de rentre le débit (en Mbps) du GS</t>
   </si>
 </sst>
 </file>
@@ -995,14 +995,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1592,7 +1592,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1600,19 +1600,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="17"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="17"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1620,25 +1620,25 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="18"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="18"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="18"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1646,19 +1646,19 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="17"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1666,31 +1666,31 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="18"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="18"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="18"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="18"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1698,19 +1698,19 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="17"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="17"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="17"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2DAA38-DBDF-46E2-B419-F6451EE365BA}">
   <dimension ref="C2:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2016,7 +2016,7 @@
       </c>
     </row>
     <row r="6" spans="3:5" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="C6" s="19">
+      <c r="C6" s="17">
         <f t="shared" ref="C6:C9" si="0">C5+1</f>
         <v>18</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>59</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.45">
@@ -2429,7 +2429,7 @@
         <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.45">
@@ -2445,7 +2445,7 @@
         <v>68</v>
       </c>
       <c r="D60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.45">
@@ -2747,8 +2747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
   <dimension ref="A3:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3014,7 +3014,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3025,7 +3025,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="17"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
@@ -3034,7 +3034,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="17"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
@@ -3043,7 +3043,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3054,7 +3054,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
@@ -3063,7 +3063,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5" t="s">
         <v>55</v>
       </c>
@@ -3072,7 +3072,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -3083,7 +3083,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="17"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
@@ -3092,7 +3092,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
@@ -3101,7 +3101,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3112,7 +3112,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -3121,7 +3121,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
@@ -3130,7 +3130,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -3141,7 +3141,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
@@ -3150,7 +3150,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -3159,7 +3159,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
@@ -3168,7 +3168,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="17"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
@@ -3177,7 +3177,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="19" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3188,7 +3188,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
@@ -3197,7 +3197,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
@@ -3206,7 +3206,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -3215,14 +3215,14 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="17"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="17"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
save figure feature added
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A32363-0F9C-4A37-A1D6-54F51C6D311E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550090C0-8171-439A-A8AA-CDC86EDF1784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="-16320" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="4" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="219">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -853,33 +853,37 @@
     <t>Le système doit permettre à l'utilisateur de rentre le débit (en Mbps) du GS</t>
   </si>
   <si>
-    <t>Le système doit exporter les résulats dans un fichier .csv avec la nomenclature suivante :
-- Pour les POI : Result_POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan)
-- Pour les GS : Result_Ground Station visibility (Nom du Satellite-Numéro du satellite-Numéro du
-plan)
-- Pour les resultats globaux : Result_Nom de la mission</t>
-  </si>
-  <si>
     <t>Le système doit indiquer l'élévation max (en °) pour chaque passage</t>
+  </si>
+  <si>
+    <t>6 - As a user, I want to obtain simulation reports containing information on orbital parameters, 
+eclipse periods and transits over geographical areas</t>
+  </si>
+  <si>
+    <t>Le système doit exporter les graphs associés aux résultats au format .png  avec la nomenclature suivante :
+- Pour les POI :  Result Nom du POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan) Graph.png
+- Pour les GS : Result Nom de la GS visibility (Nom du Satellite-Numéro du satellite-Numéro du
+plan) Graph.png</t>
   </si>
   <si>
     <t>Le système doit exporter la trace au sol et l'orbite de la simulation au format .png 
 avec la nomenclature suivante :
-- Pour la trace au sol : Ground_Track_Nom de la mission
-- Pour l'orbite : Orbit_Nom de la mission</t>
-  </si>
-  <si>
-    <t>Le système doit exporter les graphs associés aux résultats au format .png  avec la nomenclature suivante :
-- Pour les POI :  Result_POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan)_Graph
-- Pour les GS : Result_Ground Station visibility (Nom du Satellite-Numéro du satellite-Numéro du
-plan)_Graph</t>
+- Pour la trace au sol : Ground Track Nom de la mission.png
+- Pour l'orbite : Orbit Nom de la mission.png</t>
+  </si>
+  <si>
+    <t>Le système doit exporter les résulats dans un fichier .csv avec la nomenclature suivante :
+- Pour les POI : Result POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan).csv
+- Pour les GS : Result Ground Station visibility (Nom du Satellite-Numéro du satellite-Numéro du
+plan).csv
+- Pour les resultats globaux : Result Nom de la mission.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,6 +936,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -973,7 +991,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -1020,11 +1038,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1614,7 +1636,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1622,19 +1644,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="18"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="18"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1642,25 +1664,25 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="19"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="19"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="19"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1668,19 +1690,19 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="18"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="18"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1688,31 +1710,31 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="19"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="19"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="19"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="19"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1720,19 +1742,19 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="18"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="18"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="18"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
@@ -2642,10 +2664,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
-  <dimension ref="A3:C36"/>
+  <dimension ref="A3:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2787,8 +2809,8 @@
       <c r="A20">
         <v>108</v>
       </c>
-      <c r="B20" t="s">
-        <v>215</v>
+      <c r="B20" s="18" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -2894,7 +2916,7 @@
         <v>119</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="57" x14ac:dyDescent="0.45">
@@ -2902,15 +2924,20 @@
         <v>120</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A36" s="17">
         <v>121</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B37" s="21" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3071,7 +3098,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3082,7 +3109,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
@@ -3091,7 +3118,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="4" t="s">
         <v>59</v>
       </c>
@@ -3100,7 +3127,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3111,7 +3138,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
@@ -3120,7 +3147,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="5" t="s">
         <v>55</v>
       </c>
@@ -3129,7 +3156,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -3140,7 +3167,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
@@ -3149,7 +3176,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
@@ -3158,7 +3185,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3169,7 +3196,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -3178,7 +3205,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
@@ -3187,7 +3214,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -3198,7 +3225,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
@@ -3207,7 +3234,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -3216,7 +3243,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
@@ -3225,7 +3252,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
@@ -3234,7 +3261,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3245,7 +3272,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
@@ -3254,7 +3281,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
@@ -3263,7 +3290,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -3272,14 +3299,14 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="18"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Mission folder added for save feature
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D95FD21-3DE9-47EC-9B1F-5BD265DC5995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243A17D6-7E04-472D-A2BC-A3DB52580E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10035" yWindow="-13545" windowWidth="16080" windowHeight="9795" firstSheet="1" activeTab="4" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="220">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -877,6 +877,9 @@
 - Pour les POI :  Result Nom du POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan) figure.png
 - Pour les GS : Result Nom de la GS visibility (Nom du Satellite-Numéro du satellite-Numéro du
 plan) figure.png</t>
+  </si>
+  <si>
+    <t>mdp : EO_tools</t>
   </si>
 </sst>
 </file>
@@ -1556,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3161A64A-A6FA-48E0-B23C-B5A382045211}">
-  <dimension ref="B2:B25"/>
+  <dimension ref="B2:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1605,6 +1608,11 @@
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2666,8 +2674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
   <dimension ref="A3:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
xlsx and pptx updated, sun zenith angle to sza.py
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoca\Desktop\eo_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243A17D6-7E04-472D-A2BC-A3DB52580E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F898EFD-E665-43DA-8972-4F6A3FF09D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="2" activeTab="4" xr2:uid="{C958BF33-3D3E-4E58-8303-ED0CD1C2956C}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse du besoin" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="225">
   <si>
     <t>Pour la station-sol :  Définition de l’objet (arc d’orbite, élévation, volume de donnée (acquisition et vidage), les débits d’acquisition et de vidage ainsi que les opportunités d’acquisition et de vidage</t>
   </si>
@@ -866,13 +866,6 @@
 - Pour l'orbite : Orbit Nom de la mission.png</t>
   </si>
   <si>
-    <t>Le système doit exporter les résulats dans un fichier .csv avec la nomenclature suivante :
-- Pour les POI : Result POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan).csv
-- Pour les GS : Result Ground Station visibility (Nom du Satellite-Numéro du satellite-Numéro du
-plan).csv
-- Pour les resultats globaux : Result Nom de la mission.csv</t>
-  </si>
-  <si>
     <t>Le système doit exporter les graphs associés aux résultats au format .png  avec la nomenclature suivante :
 - Pour les POI :  Result Nom du POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan) figure.png
 - Pour les GS : Result Nom de la GS visibility (Nom du Satellite-Numéro du satellite-Numéro du
@@ -880,6 +873,63 @@
   </si>
   <si>
     <t>mdp : EO_tools</t>
+  </si>
+  <si>
+    <t>Le système doit exporter les résulats dans un fichier .csv avec la nomenclature suivante :
+- Pour les POI : Result POI visibility (Nom du Satellite-Numéro du satellite-Numéro du plan).csv
+- Pour les GS : Result Ground Station visibility (Nom du Satellite-Numéro du satellite-Numéro du
+plan).csv</t>
+  </si>
+  <si>
+    <t>Le logiciel doit pouvoir importer le template du rapport sous .docx, portant le nom de "Mission report Template.docx"</t>
+  </si>
+  <si>
+    <t>Le système doit exporter les données suivant dans un fichier, portant le nom suivant : "Mission report for {Mission name}", sous format .pdf: 
+- Les informations relatives à la mission
+- Les informations relatives à la constellation
+- Les informations relatives aux POI et GS</t>
+  </si>
+  <si>
+    <t>Les informations relatives à la mission sont :
+- Le nom de la mission
+- Le type de la mission
+- La durée de la mission (en jours)
+- Le SZA de la mission
+- La liste des stations sol de la mission
+- La liste des POI
+- Le nom de la constellation de la mission
+- Une carte avec l'emplacement des POI et GS</t>
+  </si>
+  <si>
+    <t>Les informations relatives à la constellation sont :
+- Le nom de la constellation
+- Le nombre de satellite
+- Le nombre de plans orbitaux
+- Le facteur de phase entre chaque plan
+- Le nom du satellite modèle
+- Le type d'orbite
+- Le semi grand axe (en km)
+- l'inclinaison (en °)
+- l'eccentricité
+- La période orbitale (en s)
+- Le nombre d'orbite par jour
+- La revisite à 0°, 45° et 60°
+- La fauché (en km)
+- L'angle de dépointage (en °)
+- La représentation 3D de l'orbite
+- La trace au sol</t>
+  </si>
+  <si>
+    <t>Les informations relatives aux POI et GS sont :
+- Le nom
+- Les coordonnées (en DD)
+- L'altitude
+- Le nombre de fois que le POI ou la GS est visible
+- La durée moyenne de visibilité
+- Graphique donnant le nombre de visibilté par satellite
+Pour la GS :
+- les characteristiques de l'antenne (bande, elevation (en °) et débit (en Mbps))
+- La taille moyenne des données envoyées/reçues</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1289,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}" name="Tableau4" displayName="Tableau4" ref="A3:C39" totalsRowShown="0">
-  <autoFilter ref="A3:C39" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}" name="Tableau4" displayName="Tableau4" ref="A3:C42" totalsRowShown="0">
+  <autoFilter ref="A3:C42" xr:uid="{B9351F40-DDF8-4307-A7ED-DC04D09DD8EB}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FB216FF5-5C23-45FE-9C7F-41D70FC25F5D}" name="ReqID"/>
     <tableColumn id="2" xr3:uid="{27152B0E-8AF8-4A79-ABBC-8FF7DDD6B3A8}" name=" "/>
@@ -1561,7 +1611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3161A64A-A6FA-48E0-B23C-B5A382045211}">
   <dimension ref="B2:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -1612,7 +1662,7 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2021,7 +2071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2DAA38-DBDF-46E2-B419-F6451EE365BA}">
   <dimension ref="C2:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
@@ -2672,15 +2722,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC885C-0795-4641-B343-9A0104313719}">
-  <dimension ref="A3:C37"/>
+  <dimension ref="A3:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="83.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -2919,12 +2969,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="A34" s="9">
         <v>119</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="57" x14ac:dyDescent="0.45">
@@ -2935,17 +2985,57 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="A36" s="17">
         <v>121</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B37" s="19" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A38" s="17">
+        <v>122</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>123</v>
+      </c>
+      <c r="B39" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A40" s="9">
+        <v>124</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
+      <c r="A41" s="9">
+        <v>125</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="17">
+        <v>126</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>